<commit_message>
after merging and running test to check validity
</commit_message>
<xml_diff>
--- a/qaautomation.xlsx
+++ b/qaautomation.xlsx
@@ -557,12 +557,12 @@
         <v>POST</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d_
-    "first_name": "Ali",_x000d__x000d__x000d__x000d_
-    "last_name": "Ahmad",_x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d_
-    "password": "12345",_x000d__x000d__x000d__x000d_
-    "confirm_password": "12345"_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d_
+    "first_name": "Ali",_x000d__x000d__x000d__x000d__x000d_
+    "last_name": "Ahmad",_x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d_
+    "password": "12345",_x000d__x000d__x000d__x000d__x000d_
+    "confirm_password": "12345"_x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D4" t="str">
@@ -586,9 +586,9 @@
         <v>POST</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d_
-    "password": "12345"_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d_
+    "password": "12345"_x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D5" t="str">

</xml_diff>

<commit_message>
after modifying the code that stores cast members in excel sheet
</commit_message>
<xml_diff>
--- a/qaautomation.xlsx
+++ b/qaautomation.xlsx
@@ -557,12 +557,12 @@
         <v>POST</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d_
-    "first_name": "Ali",_x000d__x000d__x000d__x000d__x000d__x000d_
-    "last_name": "Ahmad",_x000d__x000d__x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d_
-    "password": "12345",_x000d__x000d__x000d__x000d__x000d__x000d_
-    "confirm_password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "first_name": "Ali",_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "last_name": "Ahmad",_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "password": "12345",_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "confirm_password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D4" t="str">
@@ -586,9 +586,9 @@
         <v>POST</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d_
-    "password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D5" t="str">
@@ -1376,6 +1376,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError numberStoredAsText="1" sqref="A1:C50"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
before making seperate read and write xlsx functions
</commit_message>
<xml_diff>
--- a/qaautomation.xlsx
+++ b/qaautomation.xlsx
@@ -558,12 +558,12 @@
         <v>POST</v>
       </c>
       <c r="C4" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "first_name": "Ali",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "last_name": "Ahmad",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "password": "12345",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "confirm_password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "first_name": "Ali",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "last_name": "Ahmad",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "password": "12345",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "confirm_password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D4" t="str">
@@ -587,9 +587,9 @@
         <v>POST</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
-    "password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">{_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "email": "ali.ahmad@gmail.com",_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
+    "password": "12345"_x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d__x000d_
 }</v>
       </c>
       <c r="D5" t="str">
@@ -1409,26 +1409,26 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v/>
+        <v>After Life | Netflix Official Site</v>
       </c>
       <c r="B3" t="str">
-        <v>https://www.hitc.com/en-gb/2020/04/26/after-life-dog-brandy-belong-to-ricky-gervais-netflix-anti/</v>
+        <v>https://www.netflix.com/title/80998491</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v/>
+        <v>After Life (TV Series 2019– ) - IMDb</v>
       </c>
       <c r="B4" t="str">
-        <v>https://www.denofgeek.com/tv/after-life-season-3-netflix-renewed/</v>
+        <v>https://www.imdb.com/title/tt8398600/</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v/>
+        <v>After.Life (2009) - IMDb</v>
       </c>
       <c r="B5" t="str">
-        <v>https://en.wikipedia.org/wiki/After_Life_(TV_series)</v>
+        <v>https://www.imdb.com/title/tt0838247/</v>
       </c>
     </row>
     <row r="6">
@@ -1436,55 +1436,55 @@
         <v/>
       </c>
       <c r="B6" t="str">
-        <v>https://www.rogerebert.com/reviews/afterlife-2010</v>
+        <v>https://www.hitc.com/en-gb/2020/04/26/after-life-dog-brandy-belong-to-ricky-gervais-netflix-anti/</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>After Life | Netflix Official Site</v>
+        <v/>
       </c>
       <c r="B7" t="str">
-        <v>https://www.netflix.com/title/80998491</v>
+        <v>https://www.denofgeek.com/tv/after-life-season-3-netflix-renewed/</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>After Life (TV Series 2019– ) - IMDb</v>
+        <v/>
       </c>
       <c r="B8" t="str">
-        <v>https://www.imdb.com/title/tt8398600/</v>
+        <v>https://en.wikipedia.org/wiki/After_Life_(TV_series)</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>After Life: Season 1 - Rotten Tomatoes</v>
+        <v/>
       </c>
       <c r="B9" t="str">
-        <v>https://www.rottentomatoes.com/tv/after_life/s01</v>
+        <v>https://www.rogerebert.com/reviews/afterlife-2010</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>After Life - Rotten Tomatoes</v>
+        <v>After Life: Season 1 - Rotten Tomatoes</v>
       </c>
       <c r="B10" t="str">
-        <v>https://www.rottentomatoes.com/tv/after_life</v>
+        <v>https://www.rottentomatoes.com/tv/after_life/s01</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Ricky Gervais calls After Life the best thing he's done. This is ...</v>
+        <v>After Life - Rotten Tomatoes</v>
       </c>
       <c r="B11" t="str">
-        <v>https://www.theguardian.com/tv-and-radio/2019/mar/11/ricky-gervais-calls-after-life-the-best-thing-hes-done-this-is-patently-false</v>
+        <v>https://www.rottentomatoes.com/tv/after_life</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>After Life season 3 release date | Netflix trailer, cast, plot ...</v>
+        <v>Ricky Gervais calls After Life the best thing he's done. This is ...</v>
       </c>
       <c r="B12" t="str">
-        <v>https://www.radiotimes.com/news/on-demand/2020-07-24/after-life-season-3-release-date/</v>
+        <v>https://www.theguardian.com/tv-and-radio/2019/mar/11/ricky-gervais-calls-after-life-the-best-thing-hes-done-this-is-patently-false</v>
       </c>
     </row>
     <row r="13">

</xml_diff>